<commit_message>
Print server details in console based on the env var -DprintDetails
</commit_message>
<xml_diff>
--- a/Spring_Boot_Features_Links.xlsx
+++ b/Spring_Boot_Features_Links.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="413">
   <si>
     <t xml:space="preserve">Task Type</t>
   </si>
@@ -92,6 +92,9 @@
   <si>
     <t xml:space="preserve">Database and Tables creation scripts for basic following modules are ready:
 - OFDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLYWAY is used</t>
   </si>
   <si>
     <t xml:space="preserve">Project Setup Documentation</t>
@@ -105,7 +108,8 @@
 4. Welcome Page </t>
   </si>
   <si>
-    <t xml:space="preserve">Google Drive Folder: \MyWork\SuperMarket\project-documents</t>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=kaxrn_n7Jsg
+Google Drive Folder: \MyWork\SuperMarket\project-documents</t>
   </si>
   <si>
     <t xml:space="preserve">Health Check</t>
@@ -2045,9 +2049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1426680</xdr:colOff>
+      <xdr:colOff>1426320</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2061,7 +2065,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="28440" y="8655480"/>
-          <a:ext cx="1398240" cy="274320"/>
+          <a:ext cx="1397880" cy="273960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2082,9 +2086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1417320</xdr:colOff>
+      <xdr:colOff>1416960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>437400</xdr:rowOff>
+      <xdr:rowOff>437040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2098,7 +2102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="16491600"/>
-          <a:ext cx="1417320" cy="264960"/>
+          <a:ext cx="1416960" cy="264600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2127,10 +2131,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.74"/>
@@ -2279,7 +2283,9 @@
       <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -2300,7 +2306,7 @@
     <row r="5" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>11</v>
@@ -2310,10 +2316,10 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -2335,7 +2341,7 @@
     <row r="6" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>11</v>
@@ -2345,10 +2351,10 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -2370,7 +2376,7 @@
     <row r="7" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>11</v>
@@ -2381,7 +2387,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="2"/>
       <c r="I7" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -2403,17 +2409,17 @@
     <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
@@ -2436,10 +2442,10 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="7"/>
@@ -2466,10 +2472,10 @@
     </row>
     <row r="10" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>11</v>
@@ -2479,7 +2485,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="9"/>
@@ -2501,10 +2507,10 @@
     </row>
     <row r="11" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>11</v>
@@ -2514,10 +2520,10 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -2539,7 +2545,7 @@
     <row r="12" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>11</v>
@@ -2549,10 +2555,10 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -2574,7 +2580,7 @@
     <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>11</v>
@@ -2584,7 +2590,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="9"/>
@@ -2607,7 +2613,7 @@
     <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>11</v>
@@ -2617,7 +2623,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="9"/>
@@ -2640,7 +2646,7 @@
     <row r="15" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>11</v>
@@ -2650,7 +2656,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="9"/>
@@ -2673,7 +2679,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>11</v>
@@ -2683,10 +2689,10 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -2708,7 +2714,7 @@
     <row r="17" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>11</v>
@@ -2718,10 +2724,10 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -2743,7 +2749,7 @@
     <row r="18" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>11</v>
@@ -2753,10 +2759,10 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -2778,7 +2784,7 @@
     <row r="19" customFormat="false" ht="219.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>11</v>
@@ -2788,10 +2794,10 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -2813,7 +2819,7 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>11</v>
@@ -2823,7 +2829,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="9"/>
@@ -2846,7 +2852,7 @@
     <row r="21" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>11</v>
@@ -2856,10 +2862,10 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -2881,7 +2887,7 @@
     <row r="22" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>11</v>
@@ -2891,10 +2897,10 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -2916,7 +2922,7 @@
     <row r="23" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>11</v>
@@ -2926,10 +2932,10 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -2951,17 +2957,17 @@
     <row r="24" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="9"/>
@@ -2985,7 +2991,7 @@
     <row r="25" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>11</v>
@@ -2996,7 +3002,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="2"/>
       <c r="I25" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -3018,7 +3024,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>11</v>
@@ -3030,10 +3036,10 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -3055,7 +3061,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>11</v>
@@ -3067,7 +3073,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="9"/>
@@ -3090,7 +3096,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>11</v>
@@ -3100,7 +3106,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="9"/>
@@ -3123,7 +3129,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>11</v>
@@ -3133,7 +3139,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="9"/>
@@ -3156,7 +3162,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>11</v>
@@ -3166,10 +3172,10 @@
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
@@ -3190,10 +3196,10 @@
     </row>
     <row r="31" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>11</v>
@@ -3205,10 +3211,10 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -3230,7 +3236,7 @@
     <row r="32" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>11</v>
@@ -3242,10 +3248,10 @@
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -3267,7 +3273,7 @@
     <row r="33" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>11</v>
@@ -3279,10 +3285,10 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -3304,7 +3310,7 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>11</v>
@@ -3314,7 +3320,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="9"/>
@@ -3337,7 +3343,7 @@
     <row r="35" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>11</v>
@@ -3349,10 +3355,10 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
@@ -3374,7 +3380,7 @@
     <row r="36" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>11</v>
@@ -3386,10 +3392,10 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
@@ -3410,10 +3416,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
@@ -3441,23 +3447,23 @@
     </row>
     <row r="38" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -3479,17 +3485,17 @@
     <row r="39" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="9"/>
@@ -3512,10 +3518,10 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="7"/>
@@ -3542,10 +3548,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>11</v>
@@ -3578,7 +3584,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>11</v>
@@ -3589,7 +3595,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="3"/>
       <c r="I42" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -3611,7 +3617,7 @@
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>11</v>
@@ -3644,7 +3650,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>11</v>
@@ -3677,7 +3683,7 @@
     <row r="45" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>11</v>
@@ -3687,10 +3693,10 @@
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
       <c r="H45" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -3712,7 +3718,7 @@
     <row r="46" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>11</v>
@@ -3743,7 +3749,7 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
       <c r="B47" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>11</v>
@@ -3774,7 +3780,7 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
       <c r="B48" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>11</v>
@@ -3785,7 +3791,7 @@
       <c r="G48" s="18"/>
       <c r="H48" s="3"/>
       <c r="I48" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -3807,7 +3813,7 @@
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
       <c r="B49" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>11</v>
@@ -3837,10 +3843,10 @@
     </row>
     <row r="50" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>11</v>
@@ -3852,10 +3858,10 @@
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -3877,7 +3883,7 @@
     <row r="51" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
       <c r="B51" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>11</v>
@@ -3888,13 +3894,13 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -3917,7 +3923,7 @@
     <row r="52" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="19"/>
       <c r="B52" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>11</v>
@@ -3929,10 +3935,10 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -3953,10 +3959,10 @@
     </row>
     <row r="53" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>11</v>
@@ -3966,10 +3972,10 @@
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
       <c r="H53" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -3991,7 +3997,7 @@
     <row r="54" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>11</v>
@@ -4001,10 +4007,10 @@
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -4026,10 +4032,10 @@
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
       <c r="B55" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="7"/>
@@ -4057,17 +4063,17 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I56" s="8"/>
       <c r="J56" s="9"/>
@@ -4089,10 +4095,10 @@
     </row>
     <row r="57" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>11</v>
@@ -4125,7 +4131,7 @@
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>11</v>
@@ -4138,7 +4144,7 @@
       <c r="G58" s="7"/>
       <c r="H58" s="3"/>
       <c r="I58" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -4160,7 +4166,7 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
       <c r="B59" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>11</v>
@@ -4193,7 +4199,7 @@
     <row r="60" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
       <c r="B60" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>11</v>
@@ -4205,10 +4211,10 @@
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -4230,7 +4236,7 @@
     <row r="61" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
       <c r="B61" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>11</v>
@@ -4242,7 +4248,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I61" s="11"/>
       <c r="J61" s="9"/>
@@ -4266,7 +4272,7 @@
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
       <c r="B62" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>11</v>
@@ -4278,7 +4284,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
       <c r="H62" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I62" s="8"/>
       <c r="J62" s="9"/>
@@ -4300,10 +4306,10 @@
     </row>
     <row r="63" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>11</v>
@@ -4315,7 +4321,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I63" s="8"/>
       <c r="J63" s="9"/>
@@ -4338,7 +4344,7 @@
     <row r="64" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
       <c r="B64" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>11</v>
@@ -4350,7 +4356,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I64" s="8"/>
       <c r="J64" s="9"/>
@@ -4374,17 +4380,17 @@
     <row r="65" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
       <c r="B65" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
       <c r="H65" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I65" s="8"/>
       <c r="J65" s="9"/>
@@ -4407,7 +4413,7 @@
     <row r="66" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
       <c r="B66" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>11</v>
@@ -4417,7 +4423,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
       <c r="H66" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I66" s="8"/>
       <c r="J66" s="9"/>
@@ -4440,7 +4446,7 @@
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
       <c r="B67" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>11</v>
@@ -4452,7 +4458,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
       <c r="H67" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I67" s="8"/>
       <c r="J67" s="9"/>
@@ -4475,7 +4481,7 @@
     <row r="68" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
       <c r="B68" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>11</v>
@@ -4487,7 +4493,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
       <c r="H68" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I68" s="8"/>
       <c r="J68" s="9"/>
@@ -4511,7 +4517,7 @@
     <row r="69" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3"/>
       <c r="B69" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>11</v>
@@ -4521,10 +4527,10 @@
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
       <c r="H69" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -4546,7 +4552,7 @@
     <row r="70" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
       <c r="B70" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>11</v>
@@ -4558,7 +4564,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
       <c r="H70" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I70" s="16"/>
       <c r="J70" s="9"/>
@@ -4582,10 +4588,10 @@
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
       <c r="B71" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="3"/>
@@ -4612,13 +4618,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="3"/>
@@ -4646,10 +4652,10 @@
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3"/>
       <c r="B73" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="3"/>
@@ -4677,10 +4683,10 @@
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
       <c r="B74" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="3"/>
@@ -4707,13 +4713,13 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D75" s="13"/>
       <c r="E75" s="3"/>
@@ -4740,20 +4746,20 @@
     </row>
     <row r="76" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I76" s="8"/>
       <c r="J76" s="9"/>
@@ -4776,7 +4782,7 @@
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3"/>
       <c r="B77" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C77" s="17" t="s">
         <v>11</v>
@@ -4807,10 +4813,10 @@
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
       <c r="B78" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="3"/>
@@ -4837,10 +4843,10 @@
     </row>
     <row r="79" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>11</v>
@@ -4850,10 +4856,10 @@
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -4875,7 +4881,7 @@
     <row r="80" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3"/>
       <c r="B80" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C80" s="17" t="s">
         <v>11</v>
@@ -4885,10 +4891,10 @@
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
@@ -4910,7 +4916,7 @@
     <row r="81" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3"/>
       <c r="B81" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C81" s="17" t="s">
         <v>11</v>
@@ -4920,7 +4926,7 @@
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I81" s="8"/>
       <c r="J81" s="9"/>
@@ -4943,7 +4949,7 @@
     <row r="82" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="8"/>
       <c r="B82" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C82" s="17" t="s">
         <v>11</v>
@@ -4953,10 +4959,10 @@
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
       <c r="H82" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
@@ -4977,13 +4983,13 @@
     </row>
     <row r="83" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
@@ -4991,7 +4997,7 @@
       <c r="G83" s="13"/>
       <c r="H83" s="13"/>
       <c r="I83" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
@@ -5012,13 +5018,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
@@ -5046,7 +5052,7 @@
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="8"/>
       <c r="B85" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
@@ -5075,7 +5081,7 @@
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="8"/>
       <c r="B86" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C86" s="13"/>
       <c r="D86" s="13"/>
@@ -5103,10 +5109,10 @@
     </row>
     <row r="87" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C87" s="17" t="s">
         <v>11</v>
@@ -5163,10 +5169,10 @@
     </row>
     <row r="89" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="20" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C89" s="17" t="s">
         <v>11</v>
@@ -5176,10 +5182,10 @@
       <c r="F89" s="13"/>
       <c r="G89" s="13"/>
       <c r="H89" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
@@ -5200,13 +5206,13 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
@@ -5233,13 +5239,13 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
@@ -5266,13 +5272,13 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
@@ -10705,26 +10711,27 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I11" r:id="rId1" display="http://stick2code.blogspot.com/2014/03/solved-orgspringframeworkwebhttpmediaty.html"/>
-    <hyperlink ref="I16" r:id="rId2" display="https://dzone.com/articles/7-rules-for-rest-api-uri-design-1&#10;"/>
-    <hyperlink ref="I18" r:id="rId3" display="http://www.baeldung.com/global-error-handler-in-a-spring-rest-api&#10;"/>
-    <hyperlink ref="I21" r:id="rId4" display="http://stackoverflow.com/questions/20198275/how-to-manage-rest-api-versioning-with-spring"/>
-    <hyperlink ref="I26" r:id="rId5" display="https://s3.amazonaws.com/tfpearsonecollege/bestpractices/RESTful+Best+Practices.pdf"/>
-    <hyperlink ref="I30" r:id="rId6" display="https://www.infosys.com/digital/insights/Documents/restful-web-services.pdf"/>
-    <hyperlink ref="I32" r:id="rId7" display="https://www.petrikainulainen.net/programming/spring-framework/unit-testing-of-spring-mvc-controllers-configuration/"/>
-    <hyperlink ref="I38" r:id="rId8" display="https://stackoverflow.com/questions/20143401/how-to-analyze-a-jmeter-summary-report"/>
-    <hyperlink ref="I42" r:id="rId9" display="https://www.java-success.com/spring-javaconfig-configuration-and-transactionmanager/"/>
-    <hyperlink ref="I48" r:id="rId10" display="https://www.thoughts-on-java.org/hibernate-logging-guide/"/>
-    <hyperlink ref="I50" r:id="rId11" display="https://www.baeldung.com/spring-yaml&#10;&#10;https://www.concretepage.com/spring-boot/spring-boot-profiles-example"/>
-    <hyperlink ref="G51" r:id="rId12" display="https://www.callicoder.com/spring-boot-configuration-properties-example/&#10;&#10;https://www.youtube.com/watch?v=0G9X-pTv_UU&#10;&#10;https://www.concretepage.com/spring-boot/spring-boot-profiles-example"/>
-    <hyperlink ref="I51" r:id="rId13" display="https://www.callicoder.com/spring-boot-configuration-properties-example/&#10;&#10;https://www.youtube.com/watch?v=0G9X-pTv_UU"/>
-    <hyperlink ref="I52" r:id="rId14" display="https://www.javacodegeeks.com/2014/09/using-configurationproperties-in-spring-boot.html"/>
-    <hyperlink ref="I58" r:id="rId15" display="http://www.baeldung.com/validation-angularjs-spring-mvc"/>
-    <hyperlink ref="I60" r:id="rId16" display="http://plnkr.co/edit/xmjmIId0c9Glh5QH97xz?p=preview (Pagination)&#10;https://docs.angularjs.org/api/ng/filter/orderBy (Sorting)&#10;https://embed.plnkr.co/plunk/iP2NcF (pageSize dropdown)"/>
-    <hyperlink ref="I69" r:id="rId17" display="http://blog.restcase.com/top-5-rest-api-security-guidelines/"/>
-    <hyperlink ref="I79" r:id="rId18" display="https://www.javacodegeeks.com/2011/01/10-tips-proper-application-logging.html?utm_content=buffer1aa47&amp;utm_medium=social&amp;utm_source=twitter.com&amp;utm_campaign=buffer"/>
-    <hyperlink ref="I80" r:id="rId19" display="https://logback.qos.ch/manual/mdc.html"/>
-    <hyperlink ref="I82" r:id="rId20" display="https://www.javacodegeeks.com/2014/07/how-to-instantly-improve-your-java-logging-with-7-logback-tweaks.html"/>
+    <hyperlink ref="I5" r:id="rId1" display="https://www.youtube.com/watch?v=kaxrn_n7Jsg"/>
+    <hyperlink ref="I11" r:id="rId2" display="http://stick2code.blogspot.com/2014/03/solved-orgspringframeworkwebhttpmediaty.html"/>
+    <hyperlink ref="I16" r:id="rId3" display="https://dzone.com/articles/7-rules-for-rest-api-uri-design-1&#10;"/>
+    <hyperlink ref="I18" r:id="rId4" display="http://www.baeldung.com/global-error-handler-in-a-spring-rest-api&#10;"/>
+    <hyperlink ref="I21" r:id="rId5" display="http://stackoverflow.com/questions/20198275/how-to-manage-rest-api-versioning-with-spring"/>
+    <hyperlink ref="I26" r:id="rId6" display="https://s3.amazonaws.com/tfpearsonecollege/bestpractices/RESTful+Best+Practices.pdf"/>
+    <hyperlink ref="I30" r:id="rId7" display="https://www.infosys.com/digital/insights/Documents/restful-web-services.pdf"/>
+    <hyperlink ref="I32" r:id="rId8" display="https://www.petrikainulainen.net/programming/spring-framework/unit-testing-of-spring-mvc-controllers-configuration/"/>
+    <hyperlink ref="I38" r:id="rId9" display="https://stackoverflow.com/questions/20143401/how-to-analyze-a-jmeter-summary-report"/>
+    <hyperlink ref="I42" r:id="rId10" display="https://www.java-success.com/spring-javaconfig-configuration-and-transactionmanager/"/>
+    <hyperlink ref="I48" r:id="rId11" display="https://www.thoughts-on-java.org/hibernate-logging-guide/"/>
+    <hyperlink ref="I50" r:id="rId12" display="https://www.baeldung.com/spring-yaml&#10;&#10;https://www.concretepage.com/spring-boot/spring-boot-profiles-example"/>
+    <hyperlink ref="G51" r:id="rId13" display="https://www.callicoder.com/spring-boot-configuration-properties-example/&#10;&#10;https://www.youtube.com/watch?v=0G9X-pTv_UU&#10;&#10;https://www.concretepage.com/spring-boot/spring-boot-profiles-example"/>
+    <hyperlink ref="I51" r:id="rId14" display="https://www.callicoder.com/spring-boot-configuration-properties-example/&#10;&#10;https://www.youtube.com/watch?v=0G9X-pTv_UU"/>
+    <hyperlink ref="I52" r:id="rId15" display="https://www.javacodegeeks.com/2014/09/using-configurationproperties-in-spring-boot.html"/>
+    <hyperlink ref="I58" r:id="rId16" display="http://www.baeldung.com/validation-angularjs-spring-mvc"/>
+    <hyperlink ref="I60" r:id="rId17" display="http://plnkr.co/edit/xmjmIId0c9Glh5QH97xz?p=preview (Pagination)&#10;https://docs.angularjs.org/api/ng/filter/orderBy (Sorting)&#10;https://embed.plnkr.co/plunk/iP2NcF (pageSize dropdown)"/>
+    <hyperlink ref="I69" r:id="rId18" display="http://blog.restcase.com/top-5-rest-api-security-guidelines/"/>
+    <hyperlink ref="I79" r:id="rId19" display="https://www.javacodegeeks.com/2011/01/10-tips-proper-application-logging.html?utm_content=buffer1aa47&amp;utm_medium=social&amp;utm_source=twitter.com&amp;utm_campaign=buffer"/>
+    <hyperlink ref="I80" r:id="rId20" display="https://logback.qos.ch/manual/mdc.html"/>
+    <hyperlink ref="I82" r:id="rId21" display="https://www.javacodegeeks.com/2014/07/how-to-instantly-improve-your-java-logging-with-7-logback-tweaks.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -10733,7 +10740,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -10748,7 +10755,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -10759,49 +10766,49 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="23" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="23" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="23" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="23" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="23" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10809,7 +10816,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10817,7 +10824,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10825,7 +10832,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10833,7 +10840,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10841,7 +10848,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11083,7 +11090,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.38"/>
@@ -11095,13 +11102,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>7</v>
@@ -11159,13 +11166,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -11193,13 +11200,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -11228,10 +11235,10 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23"/>
       <c r="B5" s="23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -11260,13 +11267,13 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23"/>
       <c r="B6" s="23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -11293,10 +11300,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -11325,23 +11332,23 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="26" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -11365,13 +11372,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -11399,14 +11406,14 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -11433,13 +11440,13 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -11468,10 +11475,10 @@
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23"/>
       <c r="B12" s="23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -11499,13 +11506,13 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -11534,10 +11541,10 @@
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="23" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -11565,13 +11572,13 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -11600,14 +11607,14 @@
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23"/>
       <c r="B16" s="23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -11633,13 +11640,13 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -11667,13 +11674,13 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -11702,7 +11709,7 @@
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
       <c r="B19" s="23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -11731,10 +11738,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -11763,10 +11770,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="9"/>
@@ -11795,16 +11802,16 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -11832,7 +11839,7 @@
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9"/>
       <c r="B23" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -11860,10 +11867,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -11892,13 +11899,13 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -11926,10 +11933,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -11958,10 +11965,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -11990,7 +11997,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="23" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12107,7 +12114,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="27" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -12137,13 +12144,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -12171,13 +12178,13 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -12205,10 +12212,10 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -12237,14 +12244,14 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="22" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -12271,16 +12278,16 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -12307,14 +12314,14 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="22" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
@@ -12341,10 +12348,10 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -12373,10 +12380,10 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -12405,10 +12412,10 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
@@ -12437,10 +12444,10 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
@@ -12469,10 +12476,10 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -12501,10 +12508,10 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -12533,10 +12540,10 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
@@ -12565,10 +12572,10 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>283</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>282</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -12597,10 +12604,10 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
@@ -12629,10 +12636,10 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -12661,7 +12668,7 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -12691,16 +12698,16 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
@@ -12727,14 +12734,14 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="22" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
@@ -12761,10 +12768,10 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -12793,10 +12800,10 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -12825,12 +12832,12 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="28" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
@@ -18483,7 +18490,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.25"/>
@@ -18494,13 +18501,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
@@ -18528,7 +18535,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -18558,20 +18565,20 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="24" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -18597,13 +18604,13 @@
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23"/>
       <c r="B4" s="23" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="23" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -18629,13 +18636,13 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23"/>
       <c r="B5" s="23" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="23" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -18661,13 +18668,13 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23"/>
       <c r="B6" s="23" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="23" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -18697,7 +18704,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="23" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -18727,7 +18734,7 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="23" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -18752,7 +18759,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -18782,10 +18789,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -18814,7 +18821,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -18844,7 +18851,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -18874,7 +18881,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B13" s="29" t="str">
         <f aca="false">HYPERLINK("http://www.quizover.com/flashcards/what-does-cohesion-mean","http://www.quizover.com/flashcards/what-does-cohesion-mean")</f>
@@ -18907,7 +18914,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -18937,10 +18944,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -18969,7 +18976,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -19000,7 +19007,7 @@
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
       <c r="B17" s="23" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -19030,7 +19037,7 @@
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
       <c r="B18" s="23" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -19060,7 +19067,7 @@
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
       <c r="B19" s="23" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -19090,7 +19097,7 @@
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
       <c r="B20" s="23" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -19120,7 +19127,7 @@
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9"/>
       <c r="B21" s="23" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -19150,7 +19157,7 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9"/>
       <c r="B22" s="23" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -19207,10 +19214,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -24859,7 +24866,7 @@
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.87"/>
@@ -24870,76 +24877,76 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23"/>
       <c r="B8" s="23" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23"/>
       <c r="B9" s="23" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23"/>
       <c r="B11" s="23" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24949,64 +24956,64 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -25234,7 +25241,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="14.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="13" style="0" width="17.25"/>
@@ -25242,7 +25249,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -25268,7 +25275,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -25294,7 +25301,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -25321,7 +25328,7 @@
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="23" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -25347,7 +25354,7 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="23" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -25372,7 +25379,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -25398,7 +25405,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>

</xml_diff>